<commit_message>
made range dependent on length of contract list entries, also added comments
</commit_message>
<xml_diff>
--- a/ExcelSummary/_FGT Summary.xlsx
+++ b/ExcelSummary/_FGT Summary.xlsx
@@ -61,7 +61,7 @@
     <t>see proposed changes</t>
   </si>
   <si>
-    <t>__Blank Non-HS Template.xlsm</t>
+    <t>__Blank Non-HomeShare Template.xlsm</t>
   </si>
   <si>
     <t>Non-Residential</t>
@@ -455,7 +455,7 @@
         <v>13</v>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
         <v>0.0956</v>
@@ -467,7 +467,7 @@
         <v>0.02765</v>
       </c>
       <c r="G2" t="n">
-        <v>0.12</v>
+        <v>0.16</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -478,7 +478,7 @@
       </c>
       <c r="K2" t="n"/>
       <c r="L2" t="n">
-        <v>1408.05880191228</v>
+        <v>1883.13423588304</v>
       </c>
     </row>
     <row r="3" spans="1:12">

</xml_diff>